<commit_message>
loop among xls files  and check data  sheet name
</commit_message>
<xml_diff>
--- a/Leerplanillacupos/data/010324.xlsx
+++ b/Leerplanillacupos/data/010324.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Python\planillaCupos\Leerplanillacupos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gastonmousques/workspace/ExcelExporter/excelconverter/Leerplanillacupos/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59217B5-F72B-49FA-8443-9FA03808A173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B511D5-0BC1-1249-9998-AEB18CCA7CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27855" yWindow="3915" windowWidth="21600" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30320" yWindow="3920" windowWidth="21600" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TDICTADO.RPT" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TDICTADO.RPT!$B$1:$I$244</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$B$1:$I$244</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1893,7 +1893,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1903,6 +1903,7 @@
       <sz val="9.85"/>
       <color indexed="8"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9.85"/>
@@ -2046,7 +2047,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2368,16 +2369,16 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.796875" customWidth="1"/>
+    <col min="7" max="7" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9">
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2403,7 +2404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9">
       <c r="B2" s="7">
         <v>67928</v>
       </c>
@@ -2429,7 +2430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9">
       <c r="B3" s="7">
         <v>68035</v>
       </c>
@@ -2455,7 +2456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9">
       <c r="B4" s="7">
         <v>67929</v>
       </c>
@@ -2481,7 +2482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9">
       <c r="B5" s="7">
         <v>68037</v>
       </c>
@@ -2507,7 +2508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9">
       <c r="B6" s="7">
         <v>68038</v>
       </c>
@@ -2533,7 +2534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9">
       <c r="B7" s="7">
         <v>68039</v>
       </c>
@@ -2559,7 +2560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9">
       <c r="B8" s="7">
         <v>67931</v>
       </c>
@@ -2585,7 +2586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9">
       <c r="B9" s="7">
         <v>68040</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9">
       <c r="B10" s="7">
         <v>68060</v>
       </c>
@@ -2637,7 +2638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9">
       <c r="B11" s="7">
         <v>68061</v>
       </c>
@@ -2663,7 +2664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9">
       <c r="B12" s="7">
         <v>68062</v>
       </c>
@@ -2689,7 +2690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9">
       <c r="B13" s="7">
         <v>67972</v>
       </c>
@@ -2715,7 +2716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9">
       <c r="B14" s="7">
         <v>68089</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9">
       <c r="B15" s="7">
         <v>68090</v>
       </c>
@@ -2767,7 +2768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9">
       <c r="B16" s="7">
         <v>68091</v>
       </c>
@@ -2793,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9">
       <c r="B17" s="7">
         <v>68092</v>
       </c>
@@ -2819,7 +2820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9">
       <c r="B18" s="7">
         <v>68102</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9">
       <c r="B19" s="7">
         <v>68905</v>
       </c>
@@ -2871,7 +2872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9">
       <c r="B20" s="7">
         <v>68772</v>
       </c>
@@ -2897,7 +2898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9">
       <c r="B21" s="7">
         <v>68800</v>
       </c>
@@ -2923,7 +2924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9">
       <c r="B22" s="7">
         <v>68998</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9">
       <c r="B23" s="7">
         <v>68128</v>
       </c>
@@ -2975,7 +2976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9">
       <c r="B24" s="7">
         <v>68129</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9">
       <c r="B25" s="7">
         <v>68130</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9">
       <c r="B26" s="7">
         <v>68996</v>
       </c>
@@ -3053,7 +3054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9">
       <c r="B27" s="7">
         <v>68054</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9">
       <c r="B28" s="7">
         <v>68056</v>
       </c>
@@ -3105,7 +3106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9">
       <c r="B29" s="7">
         <v>68057</v>
       </c>
@@ -3131,7 +3132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9">
       <c r="B30" s="7">
         <v>68058</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9">
       <c r="B31" s="7">
         <v>68059</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9">
       <c r="B32" s="7">
         <v>68144</v>
       </c>
@@ -3209,7 +3210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9">
       <c r="B33" s="7">
         <v>68713</v>
       </c>
@@ -3235,7 +3236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9">
       <c r="B34" s="7">
         <v>68137</v>
       </c>
@@ -3261,7 +3262,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9">
       <c r="B35" s="7">
         <v>68138</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9">
       <c r="B36" s="7">
         <v>68139</v>
       </c>
@@ -3313,7 +3314,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9">
       <c r="B37" s="7">
         <v>67964</v>
       </c>
@@ -3339,7 +3340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9">
       <c r="B38" s="7">
         <v>67965</v>
       </c>
@@ -3365,7 +3366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9">
       <c r="B39" s="7">
         <v>67966</v>
       </c>
@@ -3391,7 +3392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9">
       <c r="B40" s="7">
         <v>68246</v>
       </c>
@@ -3417,7 +3418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9">
       <c r="B41" s="7">
         <v>68281</v>
       </c>
@@ -3443,7 +3444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9">
       <c r="B42" s="7">
         <v>67932</v>
       </c>
@@ -3469,7 +3470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9">
       <c r="B43" s="7">
         <v>67933</v>
       </c>
@@ -3495,7 +3496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9">
       <c r="B44" s="7">
         <v>67934</v>
       </c>
@@ -3521,7 +3522,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:9">
       <c r="B45" s="7">
         <v>68068</v>
       </c>
@@ -3547,7 +3548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:9">
       <c r="B46" s="7">
         <v>67935</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:9">
       <c r="B47" s="7">
         <v>68069</v>
       </c>
@@ -3599,7 +3600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9">
       <c r="B48" s="7">
         <v>67946</v>
       </c>
@@ -3625,7 +3626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9">
       <c r="B49" s="7">
         <v>68079</v>
       </c>
@@ -3651,7 +3652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9">
       <c r="B50" s="7">
         <v>68080</v>
       </c>
@@ -3677,7 +3678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9">
       <c r="B51" s="7">
         <v>68081</v>
       </c>
@@ -3703,7 +3704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9">
       <c r="B52" s="7">
         <v>68082</v>
       </c>
@@ -3729,7 +3730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9">
       <c r="B53" s="7">
         <v>67947</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9">
       <c r="B54" s="7">
         <v>68099</v>
       </c>
@@ -3781,7 +3782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9">
       <c r="B55" s="7">
         <v>67967</v>
       </c>
@@ -3807,7 +3808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9">
       <c r="B56" s="7">
         <v>68262</v>
       </c>
@@ -3833,7 +3834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:9">
       <c r="B57" s="7">
         <v>68299</v>
       </c>
@@ -3859,7 +3860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:9">
       <c r="B58" s="7">
         <v>68259</v>
       </c>
@@ -3885,7 +3886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:9">
       <c r="B59" s="7">
         <v>68258</v>
       </c>
@@ -3911,7 +3912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:9">
       <c r="B60" s="7">
         <v>68293</v>
       </c>
@@ -3937,7 +3938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:9">
       <c r="B61" s="7">
         <v>68249</v>
       </c>
@@ -3963,7 +3964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:9">
       <c r="B62" s="7">
         <v>68278</v>
       </c>
@@ -3989,7 +3990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:9">
       <c r="B63" s="7">
         <v>68762</v>
       </c>
@@ -4015,7 +4016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:9">
       <c r="B64" s="7">
         <v>68760</v>
       </c>
@@ -4041,7 +4042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:9">
       <c r="B65" s="7">
         <v>67944</v>
       </c>
@@ -4067,7 +4068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:9">
       <c r="B66" s="7">
         <v>68075</v>
       </c>
@@ -4093,7 +4094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:9">
       <c r="B67" s="7">
         <v>68076</v>
       </c>
@@ -4119,7 +4120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:9">
       <c r="B68" s="7">
         <v>68077</v>
       </c>
@@ -4145,7 +4146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:9">
       <c r="B69" s="7">
         <v>68078</v>
       </c>
@@ -4171,7 +4172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:9">
       <c r="B70" s="7">
         <v>67945</v>
       </c>
@@ -4197,7 +4198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:9">
       <c r="B71" s="7">
         <v>68098</v>
       </c>
@@ -4223,7 +4224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:9">
       <c r="B72" s="7">
         <v>67953</v>
       </c>
@@ -4249,7 +4250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:9">
       <c r="B73" s="7">
         <v>68910</v>
       </c>
@@ -4275,7 +4276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:9">
       <c r="B74" s="7">
         <v>68107</v>
       </c>
@@ -4301,7 +4302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:9">
       <c r="B75" s="7">
         <v>67955</v>
       </c>
@@ -4327,7 +4328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:9">
       <c r="B76" s="7">
         <v>68108</v>
       </c>
@@ -4353,7 +4354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:9">
       <c r="B77" s="7">
         <v>68761</v>
       </c>
@@ -4379,7 +4380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:9">
       <c r="B78" s="7">
         <v>67973</v>
       </c>
@@ -4405,7 +4406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:9">
       <c r="B79" s="7">
         <v>68146</v>
       </c>
@@ -4431,7 +4432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:9">
       <c r="B80" s="7">
         <v>68776</v>
       </c>
@@ -4457,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:9">
       <c r="B81" s="7">
         <v>68775</v>
       </c>
@@ -4483,7 +4484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:9">
       <c r="B82" s="7">
         <v>68778</v>
       </c>
@@ -4509,7 +4510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:9">
       <c r="B83" s="7">
         <v>68887</v>
       </c>
@@ -4535,7 +4536,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="84" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:9">
       <c r="B84" s="7">
         <v>68888</v>
       </c>
@@ -4561,7 +4562,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="85" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:9">
       <c r="B85" s="7">
         <v>68889</v>
       </c>
@@ -4587,7 +4588,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="86" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:9">
       <c r="B86" s="7">
         <v>68890</v>
       </c>
@@ -4613,7 +4614,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="87" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:9">
       <c r="B87" s="7">
         <v>68891</v>
       </c>
@@ -4639,7 +4640,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="88" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:9">
       <c r="B88" s="7">
         <v>68892</v>
       </c>
@@ -4665,7 +4666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:9">
       <c r="B89" s="7">
         <v>68893</v>
       </c>
@@ -4691,7 +4692,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="90" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:9">
       <c r="B90" s="7">
         <v>68894</v>
       </c>
@@ -4717,7 +4718,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="91" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:9">
       <c r="B91" s="7">
         <v>68895</v>
       </c>
@@ -4743,7 +4744,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="92" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:9">
       <c r="B92" s="7">
         <v>68896</v>
       </c>
@@ -4769,7 +4770,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="93" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:9">
       <c r="B93" s="7">
         <v>68897</v>
       </c>
@@ -4795,7 +4796,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="94" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:9">
       <c r="B94" s="7">
         <v>67975</v>
       </c>
@@ -4821,7 +4822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:9">
       <c r="B95" s="7">
         <v>68745</v>
       </c>
@@ -4847,7 +4848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:9">
       <c r="B96" s="7">
         <v>68798</v>
       </c>
@@ -4873,7 +4874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:9">
       <c r="B97" s="7">
         <v>68250</v>
       </c>
@@ -4899,7 +4900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:9">
       <c r="B98" s="7">
         <v>68279</v>
       </c>
@@ -4925,7 +4926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:9">
       <c r="B99" s="7">
         <v>68025</v>
       </c>
@@ -4951,7 +4952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:9">
       <c r="B100" s="7">
         <v>68026</v>
       </c>
@@ -4977,7 +4978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:9">
       <c r="B101" s="7">
         <v>68028</v>
       </c>
@@ -5003,7 +5004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:9">
       <c r="B102" s="7">
         <v>67971</v>
       </c>
@@ -5029,7 +5030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:9">
       <c r="B103" s="7">
         <v>67937</v>
       </c>
@@ -5055,7 +5056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:9">
       <c r="B104" s="7">
         <v>67938</v>
       </c>
@@ -5081,7 +5082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:9">
       <c r="B105" s="7">
         <v>67939</v>
       </c>
@@ -5107,7 +5108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:9">
       <c r="B106" s="7">
         <v>68063</v>
       </c>
@@ -5133,7 +5134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:9">
       <c r="B107" s="7">
         <v>67940</v>
       </c>
@@ -5159,7 +5160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:9">
       <c r="B108" s="7">
         <v>68064</v>
       </c>
@@ -5185,7 +5186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:9">
       <c r="B109" s="7">
         <v>68247</v>
       </c>
@@ -5211,7 +5212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:9">
       <c r="B110" s="7">
         <v>68282</v>
       </c>
@@ -5237,7 +5238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:9">
       <c r="B111" s="7">
         <v>68029</v>
       </c>
@@ -5263,7 +5264,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:9">
       <c r="B112" s="7">
         <v>68030</v>
       </c>
@@ -5289,7 +5290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:9">
       <c r="B113" s="7">
         <v>68031</v>
       </c>
@@ -5315,7 +5316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:9">
       <c r="B114" s="7">
         <v>69280</v>
       </c>
@@ -5341,7 +5342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:9">
       <c r="B115" s="7">
         <v>67924</v>
       </c>
@@ -5367,7 +5368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:9">
       <c r="B116" s="7">
         <v>67925</v>
       </c>
@@ -5393,7 +5394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:9">
       <c r="B117" s="7">
         <v>67927</v>
       </c>
@@ -5419,7 +5420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:9">
       <c r="B118" s="7">
         <v>68253</v>
       </c>
@@ -5445,7 +5446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:9">
       <c r="B119" s="7">
         <v>68288</v>
       </c>
@@ -5471,7 +5472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:9">
       <c r="B120" s="7">
         <v>68252</v>
       </c>
@@ -5497,7 +5498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:9">
       <c r="B121" s="7">
         <v>68287</v>
       </c>
@@ -5523,7 +5524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:9">
       <c r="B122" s="7">
         <v>68295</v>
       </c>
@@ -5549,7 +5550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:9">
       <c r="B123" s="7">
         <v>68296</v>
       </c>
@@ -5575,7 +5576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:9">
       <c r="B124" s="7">
         <v>68213</v>
       </c>
@@ -5601,7 +5602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:9">
       <c r="B125" s="7">
         <v>68214</v>
       </c>
@@ -5627,7 +5628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:9">
       <c r="B126" s="7">
         <v>68132</v>
       </c>
@@ -5653,7 +5654,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:9">
       <c r="B127" s="7">
         <v>68133</v>
       </c>
@@ -5679,7 +5680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:9">
       <c r="B128" s="7">
         <v>67974</v>
       </c>
@@ -5705,7 +5706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:9">
       <c r="B129" s="7">
         <v>68131</v>
       </c>
@@ -5731,7 +5732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:9">
       <c r="B130" s="7">
         <v>68140</v>
       </c>
@@ -5757,7 +5758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:9">
       <c r="B131" s="7">
         <v>68141</v>
       </c>
@@ -5783,7 +5784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:9">
       <c r="B132" s="7">
         <v>68142</v>
       </c>
@@ -5809,7 +5810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:9">
       <c r="B133" s="7">
         <v>68773</v>
       </c>
@@ -5835,7 +5836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:9">
       <c r="B134" s="7">
         <v>68256</v>
       </c>
@@ -5861,7 +5862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:9">
       <c r="B135" s="7">
         <v>68145</v>
       </c>
@@ -5887,7 +5888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:9">
       <c r="B136" s="7">
         <v>68714</v>
       </c>
@@ -5913,7 +5914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:9">
       <c r="B137" s="7">
         <v>67950</v>
       </c>
@@ -5939,7 +5940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:9">
       <c r="B138" s="7">
         <v>67952</v>
       </c>
@@ -5965,7 +5966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:9">
       <c r="B139" s="7">
         <v>68104</v>
       </c>
@@ -5991,7 +5992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:9">
       <c r="B140" s="7">
         <v>67970</v>
       </c>
@@ -6017,7 +6018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:9">
       <c r="B141" s="7">
         <v>68105</v>
       </c>
@@ -6043,7 +6044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:9">
       <c r="B142" s="7">
         <v>68134</v>
       </c>
@@ -6069,7 +6070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:9">
       <c r="B143" s="7">
         <v>68135</v>
       </c>
@@ -6095,7 +6096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:9">
       <c r="B144" s="7">
         <v>68136</v>
       </c>
@@ -6121,7 +6122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:9">
       <c r="B145" s="7">
         <v>68770</v>
       </c>
@@ -6147,7 +6148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:9">
       <c r="B146" s="7">
         <v>68251</v>
       </c>
@@ -6173,7 +6174,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:9">
       <c r="B147" s="7">
         <v>68284</v>
       </c>
@@ -6199,7 +6200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:9">
       <c r="B148" s="7">
         <v>68286</v>
       </c>
@@ -6225,7 +6226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:9">
       <c r="B149" s="7">
         <v>68283</v>
       </c>
@@ -6251,7 +6252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:9">
       <c r="B150" s="7">
         <v>68285</v>
       </c>
@@ -6277,7 +6278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:9">
       <c r="B151" s="7">
         <v>68257</v>
       </c>
@@ -6303,7 +6304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:9">
       <c r="B152" s="7">
         <v>69022</v>
       </c>
@@ -6329,7 +6330,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:9">
       <c r="B153" s="7">
         <v>68292</v>
       </c>
@@ -6355,7 +6356,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:9">
       <c r="B154" s="7">
         <v>68291</v>
       </c>
@@ -6381,7 +6382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:9">
       <c r="B155" s="7">
         <v>68263</v>
       </c>
@@ -6407,7 +6408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:9">
       <c r="B156" s="7">
         <v>68300</v>
       </c>
@@ -6433,7 +6434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:9">
       <c r="B157" s="7">
         <v>68041</v>
       </c>
@@ -6459,7 +6460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:9">
       <c r="B158" s="7">
         <v>68043</v>
       </c>
@@ -6485,7 +6486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:9">
       <c r="B159" s="7">
         <v>68044</v>
       </c>
@@ -6511,7 +6512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:9">
       <c r="B160" s="7">
         <v>68045</v>
       </c>
@@ -6537,7 +6538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:9">
       <c r="B161" s="7">
         <v>68046</v>
       </c>
@@ -6563,7 +6564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:9">
       <c r="B162" s="7">
         <v>68147</v>
       </c>
@@ -6589,7 +6590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:9">
       <c r="B163" s="7">
         <v>67920</v>
       </c>
@@ -6615,7 +6616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:9">
       <c r="B164" s="7">
         <v>67921</v>
       </c>
@@ -6641,7 +6642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:9">
       <c r="B165" s="7">
         <v>67923</v>
       </c>
@@ -6667,7 +6668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:9">
       <c r="B166" s="7">
         <v>68999</v>
       </c>
@@ -6693,7 +6694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:9">
       <c r="B167" s="7">
         <v>68936</v>
       </c>
@@ -6719,7 +6720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:9">
       <c r="B168" s="7">
         <v>67958</v>
       </c>
@@ -6745,7 +6746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:9">
       <c r="B169" s="7">
         <v>67959</v>
       </c>
@@ -6771,7 +6772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:9">
       <c r="B170" s="7">
         <v>67960</v>
       </c>
@@ -6797,7 +6798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:9">
       <c r="B171" s="7">
         <v>68032</v>
       </c>
@@ -6823,7 +6824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:9">
       <c r="B172" s="7">
         <v>68033</v>
       </c>
@@ -6849,7 +6850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:9">
       <c r="B173" s="7">
         <v>68034</v>
       </c>
@@ -6875,7 +6876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:9">
       <c r="B174" s="7">
         <v>69281</v>
       </c>
@@ -6901,7 +6902,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:9">
       <c r="B175" s="7">
         <v>69557</v>
       </c>
@@ -6927,7 +6928,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:9">
       <c r="B176" s="7">
         <v>69555</v>
       </c>
@@ -6953,7 +6954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:9">
       <c r="B177" s="7">
         <v>69556</v>
       </c>
@@ -6979,7 +6980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:9">
       <c r="B178" s="7">
         <v>68254</v>
       </c>
@@ -7005,7 +7006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:9">
       <c r="B179" s="7">
         <v>68289</v>
       </c>
@@ -7031,7 +7032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:9">
       <c r="B180" s="7">
         <v>68764</v>
       </c>
@@ -7057,7 +7058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:9">
       <c r="B181" s="7">
         <v>67941</v>
       </c>
@@ -7083,7 +7084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:9">
       <c r="B182" s="7">
         <v>67942</v>
       </c>
@@ -7109,7 +7110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:9">
       <c r="B183" s="7">
         <v>67943</v>
       </c>
@@ -7135,7 +7136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:9">
       <c r="B184" s="7">
         <v>67969</v>
       </c>
@@ -7161,7 +7162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:9">
       <c r="B185" s="7">
         <v>68112</v>
       </c>
@@ -7187,7 +7188,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:9">
       <c r="B186" s="7">
         <v>68113</v>
       </c>
@@ -7213,7 +7214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:9">
       <c r="B187" s="7">
         <v>68143</v>
       </c>
@@ -7239,7 +7240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:9">
       <c r="B188" s="7">
         <v>68901</v>
       </c>
@@ -7265,7 +7266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:9">
       <c r="B189" s="7">
         <v>68766</v>
       </c>
@@ -7291,7 +7292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:9">
       <c r="B190" s="7">
         <v>68070</v>
       </c>
@@ -7317,7 +7318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:9">
       <c r="B191" s="7">
         <v>69621</v>
       </c>
@@ -7341,7 +7342,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:9">
       <c r="B192" s="7">
         <v>67916</v>
       </c>
@@ -7367,7 +7368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:9">
       <c r="B193" s="7">
         <v>68022</v>
       </c>
@@ -7393,7 +7394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:9">
       <c r="B194" s="7">
         <v>67917</v>
       </c>
@@ -7419,7 +7420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:9">
       <c r="B195" s="7">
         <v>68023</v>
       </c>
@@ -7445,7 +7446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:9">
       <c r="B196" s="7">
         <v>67919</v>
       </c>
@@ -7471,7 +7472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:9">
       <c r="B197" s="7">
         <v>68024</v>
       </c>
@@ -7497,7 +7498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:9">
       <c r="B198" s="7">
         <v>68109</v>
       </c>
@@ -7523,7 +7524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:9">
       <c r="B199" s="7">
         <v>67968</v>
       </c>
@@ -7549,7 +7550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:9">
       <c r="B200" s="7">
         <v>68110</v>
       </c>
@@ -7575,7 +7576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="201" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:9">
       <c r="B201" s="7">
         <v>68255</v>
       </c>
@@ -7601,7 +7602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:9">
       <c r="B202" s="7">
         <v>68290</v>
       </c>
@@ -7627,7 +7628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:9">
       <c r="B203" s="7">
         <v>68248</v>
       </c>
@@ -7653,7 +7654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="204" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:9">
       <c r="B204" s="7">
         <v>68298</v>
       </c>
@@ -7679,7 +7680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:9">
       <c r="B205" s="7">
         <v>68245</v>
       </c>
@@ -7705,7 +7706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:9">
       <c r="B206" s="7">
         <v>68047</v>
       </c>
@@ -7731,7 +7732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:9">
       <c r="B207" s="7">
         <v>68280</v>
       </c>
@@ -7757,7 +7758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="208" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:9">
       <c r="B208" s="7">
         <v>68049</v>
       </c>
@@ -7783,7 +7784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="209" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:9">
       <c r="B209" s="7">
         <v>68050</v>
       </c>
@@ -7809,7 +7810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="210" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:9">
       <c r="B210" s="7">
         <v>68051</v>
       </c>
@@ -7835,7 +7836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="211" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:9">
       <c r="B211" s="7">
         <v>68053</v>
       </c>
@@ -7861,7 +7862,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:9">
       <c r="B212" s="7">
         <v>67948</v>
       </c>
@@ -7887,7 +7888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="213" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:9">
       <c r="B213" s="7">
         <v>67949</v>
       </c>
@@ -7913,7 +7914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:9">
       <c r="B214" s="7">
         <v>68771</v>
       </c>
@@ -7939,7 +7940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:9">
       <c r="B215" s="7">
         <v>68780</v>
       </c>
@@ -7965,7 +7966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:9">
       <c r="B216" s="7">
         <v>67961</v>
       </c>
@@ -7991,7 +7992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="217" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:9">
       <c r="B217" s="7">
         <v>68084</v>
       </c>
@@ -8017,7 +8018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="218" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:9">
       <c r="B218" s="7">
         <v>68086</v>
       </c>
@@ -8043,7 +8044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="219" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:9">
       <c r="B219" s="7">
         <v>69527</v>
       </c>
@@ -8069,7 +8070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:9">
       <c r="B220" s="7">
         <v>68087</v>
       </c>
@@ -8095,7 +8096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="221" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:9">
       <c r="B221" s="7">
         <v>68088</v>
       </c>
@@ -8121,7 +8122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:9">
       <c r="B222" s="7">
         <v>67963</v>
       </c>
@@ -8147,7 +8148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:9">
       <c r="B223" s="7">
         <v>68100</v>
       </c>
@@ -8173,7 +8174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:9">
       <c r="B224" s="7">
         <v>68763</v>
       </c>
@@ -8199,7 +8200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:9">
       <c r="B225" s="7">
         <v>68065</v>
       </c>
@@ -8225,7 +8226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="226" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:9">
       <c r="B226" s="7">
         <v>68066</v>
       </c>
@@ -8251,7 +8252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="227" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:9">
       <c r="B227" s="7">
         <v>68067</v>
       </c>
@@ -8277,7 +8278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="228" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:9">
       <c r="B228" s="7">
         <v>67976</v>
       </c>
@@ -8303,7 +8304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:9">
       <c r="B229" s="7">
         <v>68765</v>
       </c>
@@ -8329,7 +8330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:9">
       <c r="B230" s="7">
         <v>68898</v>
       </c>
@@ -8355,7 +8356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:9">
       <c r="B231" s="7">
         <v>68935</v>
       </c>
@@ -8381,7 +8382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="232" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:9">
       <c r="B232" s="7">
         <v>68093</v>
       </c>
@@ -8407,7 +8408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:9">
       <c r="B233" s="7">
         <v>68094</v>
       </c>
@@ -8433,7 +8434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="234" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:9">
       <c r="B234" s="7">
         <v>68095</v>
       </c>
@@ -8459,7 +8460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="235" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:9">
       <c r="B235" s="7">
         <v>68096</v>
       </c>
@@ -8485,7 +8486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="236" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:9">
       <c r="B236" s="7">
         <v>68097</v>
       </c>
@@ -8511,7 +8512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="237" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:9">
       <c r="B237" s="7">
         <v>68904</v>
       </c>
@@ -8537,7 +8538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:9">
       <c r="B238" s="7">
         <v>68261</v>
       </c>
@@ -8563,7 +8564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:9">
       <c r="B239" s="7">
         <v>68779</v>
       </c>
@@ -8589,7 +8590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:9">
       <c r="B240" s="7">
         <v>68749</v>
       </c>
@@ -8615,7 +8616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="241" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:9">
       <c r="B241" s="7">
         <v>68115</v>
       </c>
@@ -8641,7 +8642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="242" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:9">
       <c r="B242" s="7">
         <v>68120</v>
       </c>
@@ -8667,7 +8668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:9">
       <c r="B243" s="7">
         <v>68260</v>
       </c>
@@ -8693,7 +8694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:9">
       <c r="B244" s="7">
         <v>68297</v>
       </c>
@@ -8719,10 +8720,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="247" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:9">
       <c r="I247" s="1"/>
     </row>
-    <row r="249" spans="2:9" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:9">
       <c r="B249" s="2"/>
       <c r="G249" s="3"/>
       <c r="H249" s="4"/>
@@ -8736,15 +8737,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100963BF6C78482F94E9C3A8CBAE1AB6B06" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="859a2229eb1d12c7746815e94b49e62d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="95c80e47-662b-4bc0-a457-b879d3f3aba4" xmlns:ns3="7f019ab0-5ffe-43e1-b2f8-62bc369ebe4f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40415db81e42c57b7ee018001e89900f" ns2:_="" ns3:_="">
     <xsd:import namespace="95c80e47-662b-4bc0-a457-b879d3f3aba4"/>
@@ -8999,6 +8991,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -9011,14 +9012,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAF1DC4D-DA7A-4EC7-AA71-BBFD4FFFD21F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A38A4BFF-C09C-4797-A1F3-EAE1B4AF10B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9037,6 +9030,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAF1DC4D-DA7A-4EC7-AA71-BBFD4FFFD21F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C07A432-C105-4508-854F-3CFD10071F1F}">
   <ds:schemaRefs>

</xml_diff>